<commit_message>
Update hns.csv with new product entries and modify scraping2.py to improve review collection logic and terminal output. Also, update hns.xlsx to reflect changes in data.
</commit_message>
<xml_diff>
--- a/hns.xlsx
+++ b/hns.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,17 +468,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Kotak kancing panjang obat diansari pernak pernik 20½ x 9 x 4 cm tebal - Tempat pernak pernik obat mur baut grosirVariasi: Diansari panjang</t>
+          <t>Eskan fresia 3 liter plastik ceret minum bening motif bungaVariasi: Eskan fresia</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>/Kotak-kancing-panjang-obat-diansari-pernak-pernik-20½-x-9-x-4-cm-tebal-Tempat-pernak-pernik-obat-mur-baut-grosir-i.145589728.7734625607</t>
+          <t>/Eskan-fresia-3-liter-plastik-ceret-minum-bening-motif-bunga-i.145589728.8605964666</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-05-03 21:01</t>
+          <t>2025-05-25 06:07</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -486,29 +486,29 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Variasi: Diansari panjang</t>
+          <t>Variasi: Eskan fresia</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Desain: baikUkuran: baikKualitas Bahan: baikSemoga cepat habis jualannya dan kembali membeli lagi ke toko ini. Terima kasih.</t>
+          <t>Ukuran: uk.kecil..sy pikir 3ltr itu besar ehtaunya datangnya malah kecil</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Celengan mini kakbah L10 P10 T15 cm - Celengan sovenir grosirVariasi: Celengan kakbah</t>
+          <t>Rak plastik serbaguna susun 3 lovina warna goldVariasi: Rak lovina Gold</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>/Celengan-mini-kakbah-L10-P10-T15-cm-Celengan-sovenir-grosir-i.145589728.28825756480</t>
+          <t>/Rak-plastik-serbaguna-susun-3-lovina-warna-gold-i.145589728.24033169934</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-05-03 20:49</t>
+          <t>2025-05-25 04:40</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,29 +516,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Variasi: Celengan kakbah</t>
+          <t>Variasi: Rak lovina Gold</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Bagus</t>
+          <t>Ukuran: pas dan sesuai</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>(10bks) korek batang kayu jadul gambar grosirVariasi: 10bks korek pelangi</t>
+          <t>Kapstok kawat vinil warna 6 gantungan - gantungan baju tempel kawatVariasi: Kapstok 6 warna</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>/(10bks)-korek-batang-kayu-jadul-gambar-grosir-i.145589728.11483476549</t>
+          <t>/Kapstok-kawat-vinil-warna-6-gantungan-gantungan-baju-tempel-kawat-i.145589728.13014371227</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-05-03 20:49</t>
+          <t>2025-05-25 01:44</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -546,29 +546,33 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Variasi: 10bks korek pelangi</t>
+          <t>Variasi: Kapstok 6 warna</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Bagus</t>
+          <t>Ssuai gmbr &amp; keterangan
+produk baik &amp; brmutu
+respon &amp; pengiriman cepat
+packing aman &amp; bgs
+Penjual amanah &amp; tr prcya</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>tempat sendok garpu alat tulis 3 ruang HDR Plast kuat tempel tembokVariasi: 3ruang HDR</t>
+          <t>Silet cukur tatra original extra tajam 10 pcs - silet serbagunaVariasi: Silet tatra</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>/tempat-sendok-garpu-alat-tulis-3-ruang-HDR-Plast-kuat-tempel-tembok-i.145589728.10242349357</t>
+          <t>/Silet-cukur-tatra-original-extra-tajam-10-pcs-silet-serbaguna-i.145589728.9915872611</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-05-03 20:49</t>
+          <t>2025-05-25 01:44</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -576,29 +580,33 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Variasi: 3ruang HDR</t>
+          <t>Variasi: Silet tatra</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Bagus</t>
+          <t>Kandungan: okKenyamanan: ck6Efek: blm dicobaSsuai gmbr &amp; keterangan
+produk baik &amp; brmutu
+respon &amp; pengiriman cepat
+packing aman &amp; bgs
+Penjual amanah &amp; tr prcya</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cetakan pastel dumpling plastik BRL tebal mengkilap ukran besar kecil miniVariasi: CETAKAN PASTEL,Besar</t>
+          <t>kipas tangan plastik karakter waru murah warna warniVariasi: Kipas bunga rotan</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>/Cetakan-pastel-dumpling-plastik-BRL-tebal-mengkilap-ukran-besar-kecil-mini-i.145589728.7747739184</t>
+          <t>/kipas-tangan-plastik-karakter-waru-murah-warna-warni-i.145589728.5337255631</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-05-03 20:49</t>
+          <t>2025-05-25 01:44</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -606,29 +614,33 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Variasi: CETAKAN PASTEL,Besar</t>
+          <t>Variasi: Kipas bunga rotan</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Bagus</t>
+          <t>Ketebalan: tebalKualitas: okDesain: menarikSsuai gmbr &amp; keterangan
+produk baik &amp; brmutu
+respon &amp; pengiriman cepat
+packing aman &amp; bgs
+Penjual amanah &amp; tr prcya</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>(12pcs) Pen bulpen Bolpenku pen lilit spiral gel murah drhop technologyVariasi: 12bj bulpenku</t>
+          <t>Rak Mini segi susun 3 Flower - Rak bumbu kosmetik serbagunaVariasi: Rak segi Flower</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>/(12pcs)-Pen-bulpen-Bolpenku-pen-lilit-spiral-gel-murah-drhop-technology-i.145589728.7516238456</t>
+          <t>/Rak-Mini-segi-susun-3-Flower-Rak-bumbu-kosmetik-serbaguna-i.145589728.21491056248</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-05-03 20:49</t>
+          <t>2025-05-25 01:08</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -636,163 +648,162 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Variasi: 12bj bulpenku</t>
+          <t>Variasi: Rak segi Flower</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Bagus</t>
+          <t>Mohon lebih d tingkatkan lg pelayanannya agar lebih teliti.. Makasih barang2 nya murah² tp berkualitas sayang nya jauh banget klo dr tempt aku mh jd ongkirnya mahal banget walaupun sdh dapet voucer gratis . Sukses terus 👍</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cangkir gelas minum plastik gmc gelas bir gagang grosirVariasi: Gelas bir plastik</t>
+          <t>(1pcs) Centong entong nasi plastik tebal warna dx termurahVariasi: Ecer_1bj centong PLG</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>/Cangkir-gelas-minum-plastik-gmc-gelas-bir-gagang-grosir-i.145589728.5581664849</t>
+          <t>/(1pcs)-Centong-entong-nasi-plastik-tebal-warna-dx-termurah-i.145589728.2821981447</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-05-03 20:49</t>
+          <t>2025-05-25 00:17</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Variasi: Gelas bir plastik</t>
+          <t>Variasi: Ecer_1bj centong PLG</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Bagus</t>
+          <t>Ketebalan: penipuDesain: penipuKualitas: penipuada 3 barang gk di kirim .. dan di paket tetep bayar full .. di chat gk di bales" .. emang sering nipu kali ni toko .. tolong yg lain mending beli di toko oren yg lain aja biar gk ketipu juga</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Basi prasmanan segi brokoli capucino plus tutup grosirVariasi: Basi segi brokoli</t>
+          <t>Gelas stand dudukan gelas oval capucino isi 6 gelas plastikVariasi: Gelas Stand Coklat</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>/Basi-prasmanan-segi-brokoli-capucino-plus-tutup-grosir-i.145589728.28054688499</t>
+          <t>/Gelas-stand-dudukan-gelas-oval-capucino-isi-6-gelas-plastik-i.145589728.19090884439</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-05-03 20:46</t>
+          <t>2025-05-24 23:51</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Variasi: Basi segi brokoli</t>
+          <t>Variasi: Gelas Stand Coklat</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Ukuran: ghjDesain: biasa ajKualitas Bahan: jelkTDK amnh</t>
+          <t>Desain: bagusKualitas Bahan: okInstalasi: mudahSangat rekomended untuk langganan</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>(isi 6pcs) Nampan loyang bulat kue sunrise 8500 plastik warna warniVariasi: Nmpn sunrise 8500,Isi 3 pcs</t>
+          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosirVariasi: Hngr benmore coklat</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>/(isi-6pcs)-Nampan-loyang-bulat-kue-sunrise-8500-plastik-warna-warni-i.145589728.25111821403</t>
+          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-05-03 20:46</t>
+          <t>2025-05-24 23:23</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Variasi: Nmpn sunrise 8500,Isi 3 pcs</t>
+          <t>Variasi: Hngr benmore coklat</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Desain: biasaKetebalan: biasaUkuran: biasaBarang yang dikirim tidak lengkap saya pesan nampan dan wakul buah ,yang datang cuma wakul buah ,nampan nya tidak dikirim , tidak amanah sekali.. tolong nampannya dikirim kak .
-Respon penjual juga tidak pernah merespon selama chek out. .</t>
+          <t>Barang sesuai pesanan.. dikemas cepat.. pengiriman cepat ,exp lama</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>wakul buah pacific coklat plastik serbagunaVariasi: Wakul buah pacific</t>
+          <t>Tong sampah segi kicik hitam 5 liter kecil persegi plastik tebalVariasi: TS. Kicik 5L HITAM,Isi 1 pcs</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>/wakul-buah-pacific-coklat-plastik-serbaguna-i.145589728.20153306191</t>
+          <t>/Tong-sampah-segi-kicik-hitam-5-liter-kecil-persegi-plastik-tebal-i.145589728.25059427941</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-05-03 20:46</t>
+          <t>2025-05-24 23:21</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Variasi: Wakul buah pacific</t>
+          <t>Variasi: TS. Kicik 5L HITAM,Isi 1 pcs</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Ukuran: bKondisi: bKualitas: bPalsuu</t>
+          <t>Desain: TopUkuran: TOPKualitas Bahan: tOPtop</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>(12pcs) Gosok jaring jala hijau cuci piring 8D grosir termurahVariasi: Lusinan jaring_8D</t>
+          <t>Piring seng enamel lurik ukuran 22 cm besar tebal merk TBVariasi: Piring seng lurik,22cm Besar</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>/(12pcs)-Gosok-jaring-jala-hijau-cuci-piring-8D-grosir-termurah-i.145589728.5215724772</t>
+          <t>/Piring-seng-enamel-lurik-ukuran-22-cm-besar-tebal-merk-TB-i.145589728.18783036648</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-05-03 20:30</t>
+          <t>2025-05-24 22:59</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Variasi: Lusinan jaring_8D</t>
+          <t>Variasi: Piring seng lurik,22cm Besar</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Kegunaan: gak nyerapKualitas Bahan: bukan benang tapi bekas saknya sayur</t>
+          <t>Ketebalan: sedangDesain: jaduuuullllllKualitas: baikTerima kasih barang sudah sampai dan sesuai</t>
         </is>
       </c>
     </row>
@@ -809,11 +820,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-05-03 20:29</t>
+          <t>2025-05-24 22:15</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -822,24 +833,24 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Ukuran: sesuaiDesain: sesuaiKondisi: baik</t>
+          <t>Ukuran: imut imutDesain: bagus warna sesuai picKondisi: dalam kondisi baikTerimakasih seller dan shopee</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Termos Capucino 6L dan 8L - Rice Ice bucket ekomonis grosirVariasi: Termos ekonomis 8L</t>
+          <t>Kursi jongkok CM Abu-abu warna tebal serbaguna - kursi duduk dapur kokohVariasi: Kursi abu ONIX</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>/Termos-Capucino-6L-dan-8L-Rice-Ice-bucket-ekomonis-grosir-i.145589728.29500951143</t>
+          <t>/Kursi-jongkok-CM-Abu-abu-warna-tebal-serbaguna-kursi-duduk-dapur-kokoh-i.145589728.7958001380</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-05-03 20:11</t>
+          <t>2025-05-24 21:01</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -847,29 +858,29 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Variasi: Termos ekonomis 8L</t>
+          <t>Variasi: Kursi abu ONIX</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Ukuran: pasDesain: okKondisi: okBarang bagus. Kualitas nya juga ok. Harga murah. Bestt bgt pokonya. Makasi ya seller. Semoga berkah</t>
+          <t>Bagus</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Gelas ukur/takar air gula tebung oval 650 ml by LS plastik grosirVariasi: Gelas ukur pipih</t>
+          <t>kapstok baju stainless 6 kait - gantungan baju stainless muranVariasi: Kapstok jempol_6</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>/Gelas-ukur-takar-air-gula-tebung-oval-650-ml-by-LS-plastik-grosir-i.145589728.6419715783</t>
+          <t>/kapstok-baju-stainless-6-kait-gantungan-baju-stainless-muran-i.145589728.6442847024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-05-03 19:47</t>
+          <t>2025-05-24 20:37</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -877,29 +888,29 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Variasi: Gelas ukur pipih</t>
+          <t>Variasi: Kapstok jempol_6</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Amanah</t>
+          <t>Desain: eleganDurabilitas: sangat bagusKualitas Bahan: kuat</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>(Isi 6pcs) Tempat kue + tutup segi WKP serbaguna higinis GrosirVariasi: Tempat kue segi WKP,Isi 6 pcs</t>
+          <t>Botol saos kecap memeclub tinggi 400 ml plastik grosirVariasi: Meme club tinggi</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>/(Isi-6pcs)-Tempat-kue-tutup-segi-WKP-serbaguna-higinis-Grosir-i.145589728.24851409448</t>
+          <t>/Botol-saos-kecap-memeclub-tinggi-400-ml-plastik-grosir-i.145589728.3913320949</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-05-03 19:16</t>
+          <t>2025-05-24 20:00</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -907,29 +918,29 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Variasi: Tempat kue segi WKP,Isi 6 pcs</t>
+          <t>Variasi: Meme club tinggi</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Desain: bagusKetebalan: lumayanKondisi Barang: baikMakasih pesanan sudah sampai dan sesuai.</t>
+          <t>Desain: bagusWarna: sesuaiKualitas: bagus</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>(12pcs) Gosok jaring jala hijau cuci piring 8D grosir termurahVariasi: Lusinan jaring_8D</t>
+          <t>kapstok baju stainless 6 kait - gantungan baju stainless muranVariasi: Kapstok jempol_6</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>/(12pcs)-Gosok-jaring-jala-hijau-cuci-piring-8D-grosir-termurah-i.145589728.5215724772</t>
+          <t>/kapstok-baju-stainless-6-kait-gantungan-baju-stainless-muran-i.145589728.6442847024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-05-03 19:15</t>
+          <t>2025-05-24 19:59</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -937,59 +948,60 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Variasi: Lusinan jaring_8D</t>
+          <t>Variasi: Kapstok jempol_6</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Kegunaan: efektifUkuran: sesuai yg dibutuhkanKualitas Bahan: awet tahan lama</t>
+          <t>Desain: bagusDurabilitas: okKualitas Bahan: kuatPuas dengan pesanan saya 
+Sesuai gambar.,.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Pengaman regulator - pengunci penahan regulator tabung gas 3 kg dan 12 kgVariasi: Pengaman</t>
+          <t>(12pcs) Cetakan roti kukus bentuk love rege cerah plastik dxVariasi: 12BJ Ctkn LOVE</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>/Pengaman-regulator-pengunci-penahan-regulator-tabung-gas-3-kg-dan-12-kg-i.145589728.2408393733</t>
+          <t>/(12pcs)-Cetakan-roti-kukus-bentuk-love-rege-cerah-plastik-dx-i.145589728.15424268542</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-05-03 18:42</t>
+          <t>2025-05-24 19:49</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Variasi: Pengaman</t>
+          <t>Variasi: 12BJ Ctkn LOVE</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Ukuran: tipisMaterial: tipis</t>
+          <t>Alhamdulillah paketku sampai dg selamat,barangnya bagus sesuai pict..makasih kak</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Termos Capucino 6L dan 8L - Rice Ice bucket ekomonis grosirVariasi: Termos ekonomis 8L</t>
+          <t>(12pak) Cotten bud - cotton bud motif bunga halus dan lembut grosirVariasi: 1pak cotenbud bunga</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>/Termos-Capucino-6L-dan-8L-Rice-Ice-bucket-ekomonis-grosir-i.145589728.29500951143</t>
+          <t>/(12pak)-Cotten-bud-cotton-bud-motif-bunga-halus-dan-lembut-grosir-i.145589728.16880893501</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-05-03 18:34</t>
+          <t>2025-05-24 19:45</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -997,29 +1009,29 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Variasi: Termos ekonomis 8L</t>
+          <t>Variasi: 1pak cotenbud bunga</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Barang datang sesuai pesanan. Pengiriman cepat terimakasih</t>
+          <t>Cocok untuk: semuaKapasitas: bagusKualitas: aman</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Piring seng enamel lurik ukuran 22 cm besar tebal merk TBVariasi: Piring seng lurik,22cm Besar</t>
+          <t>Mangkok stainless 14 cm 16 cm tebal - baskom stainless serbaguna grosirVariasi: Mangkok 16 cm</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>/Piring-seng-enamel-lurik-ukuran-22-cm-besar-tebal-merk-TB-i.145589728.18783036648</t>
+          <t>/Mangkok-stainless-14-cm-16-cm-tebal-baskom-stainless-serbaguna-grosir-i.145589728.10650960952</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-05-03 18:13</t>
+          <t>2025-05-24 19:45</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1027,29 +1039,29 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Variasi: Piring seng lurik,22cm Besar</t>
+          <t>Variasi: Mangkok 16 cm</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Ketebalan: tebalDesain: menarikKualitas: lumayan</t>
+          <t>Ukuran: yang di harapkanKualitas Bahan: bagusDurabilitas: kokoh</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Rak plastik serbaguna susun 3 lovina warna goldVariasi: Rak lovina Gold</t>
+          <t>Tambahan packing kardus paket tambahan agar safetyVariasi: Kardus saftey</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>/Rak-plastik-serbaguna-susun-3-lovina-warna-gold-i.145589728.24033169934</t>
+          <t>/Tambahan-packing-kardus-paket-tambahan-agar-safety-i.145589728.6615737043</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-05-03 18:08</t>
+          <t>2025-05-24 19:45</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1057,102 +1069,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Variasi: Rak lovina Gold</t>
+          <t>Variasi: Kardus saftey</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Alhamdulillah pesanan sudah diterima dengan baik lengkap, produk semuanya sesuai pesanan sangat puas terima kasih</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Tempat sendok weishan plus tutup higenis dan praktisVariasi: Tempat sendok wishan</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>/Tempat-sendok-weishan-plus-tutup-higenis-dan-praktis-i.145589728.20986136628</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>2025-05-03 17:59</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>5</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Variasi: Tempat sendok wishan</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Pesen macem-macem, barang datangnya lengkap dan aman, terima kasih 🙏</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>(12pak) Cotten bud - cotton bud motif bunga halus dan lembut grosirVariasi: 1pak cotenbud bunga</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>/(12pak)-Cotten-bud-cotton-bud-motif-bunga-halus-dan-lembut-grosir-i.145589728.16880893501</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>2025-05-03 17:59</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>5</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Variasi: 1pak cotenbud bunga</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Pesen macem-macem, barang datangnya lengkap dan aman, terima kasih 🙏</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Kapas selection facial cotten 100% higienis 35 gramVariasi: Kapas selection</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>/Kapas-selection-facial-cotten-100-higienis-35-gram-i.145589728.16472128299</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>2025-05-03 17:59</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>5</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Variasi: Kapas selection</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Pesen macem-macem, barang datangnya lengkap dan aman, terima kasih 🙏</t>
+          <t>Ketebalan: aman</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor scraping2.py to adjust target review count and enhance review text extraction logic. Update hns.csv with new product entries and modify hns.xlsx accordingly.
</commit_message>
<xml_diff>
--- a/hns.xlsx
+++ b/hns.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,17 +468,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Eskan fresia 3 liter plastik ceret minum bening motif bungaVariasi: Eskan fresia</t>
+          <t>Oil Jug tempat minyak sally 2 Liter plastik + TutupVariasi: Oil jug SALLY 2L</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>/Eskan-fresia-3-liter-plastik-ceret-minum-bening-motif-bunga-i.145589728.8605964666</t>
+          <t>/Oil-Jug-tempat-minyak-sally-2-Liter-plastik-Tutup-i.145589728.23248604754</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-05-25 06:07</t>
+          <t>2025-05-25 14:12</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -486,29 +486,29 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Variasi: Eskan fresia</t>
+          <t>Variasi: Oil jug SALLY 2L</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Ukuran: uk.kecil..sy pikir 3ltr itu besar ehtaunya datangnya malah kecil</t>
+          <t>Desain: menarikKualitas Bahan: tebalKualitas: baiktempat minyak nya bagus bahannya tebal kualitas nya baik muat 2 liter minyak. Desain: menarik. Kualitas Bahan: tebal. Kualitas: baik. tempat minyak nya bagus bahannya tebal kualitas nya baik muat 2 liter minyak</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rak plastik serbaguna susun 3 lovina warna goldVariasi: Rak lovina Gold</t>
+          <t>Rak Mini segi susun 3 Flower - Rak bumbu kosmetik serbagunaVariasi: Rak segi Flower</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>/Rak-plastik-serbaguna-susun-3-lovina-warna-gold-i.145589728.24033169934</t>
+          <t>/Rak-Mini-segi-susun-3-Flower-Rak-bumbu-kosmetik-serbaguna-i.145589728.21491056248</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-05-25 04:40</t>
+          <t>2025-05-25 14:10</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,29 +516,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Variasi: Rak lovina Gold</t>
+          <t>Variasi: Rak segi Flower</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Ukuran: pas dan sesuai</t>
+          <t>Ukuran: pasDesain: bagusDurabilitas: kuat dan kokoh. Ukuran: pas. Desain: bagus. Durabilitas: kuat dan kokoh</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kapstok kawat vinil warna 6 gantungan - gantungan baju tempel kawatVariasi: Kapstok 6 warna</t>
+          <t>Rak plastik serbaguna susun 3 lovina warna goldVariasi: Rak lovina Gold</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>/Kapstok-kawat-vinil-warna-6-gantungan-gantungan-baju-tempel-kawat-i.145589728.13014371227</t>
+          <t>/Rak-plastik-serbaguna-susun-3-lovina-warna-gold-i.145589728.24033169934</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-05-25 01:44</t>
+          <t>2025-05-25 14:05</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -546,16 +546,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Variasi: Kapstok 6 warna</t>
+          <t>Variasi: Rak lovina Gold</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Ssuai gmbr &amp; keterangan
-produk baik &amp; brmutu
-respon &amp; pengiriman cepat
-packing aman &amp; bgs
-Penjual amanah &amp; tr prcya</t>
+          <t>Ukuran: pas sesuai gambarKetebalan: ok tebalDurabilitas: produk sangat kuat. Ukuran: pas sesuai gambar. Ketebalan: ok tebal. Durabilitas: produk sangat kuat</t>
         </is>
       </c>
     </row>
@@ -572,11 +568,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-05-25 01:44</t>
+          <t>2025-05-25 14:00</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -585,28 +581,24 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Kandungan: okKenyamanan: ck6Efek: blm dicobaSsuai gmbr &amp; keterangan
-produk baik &amp; brmutu
-respon &amp; pengiriman cepat
-packing aman &amp; bgs
-Penjual amanah &amp; tr prcya</t>
+          <t>Produk sudah sampai sesuai dengan pesanan terimakasihhhh</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>kipas tangan plastik karakter waru murah warna warniVariasi: Kipas bunga rotan</t>
+          <t>Mangko sambal bakso tutup panda star plus sendok bulat oval plastikVariasi: Mangkok sambal tutup</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>/kipas-tangan-plastik-karakter-waru-murah-warna-warni-i.145589728.5337255631</t>
+          <t>/Mangko-sambal-bakso-tutup-panda-star-plus-sendok-bulat-oval-plastik-i.145589728.16385939181</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-05-25 01:44</t>
+          <t>2025-05-25 13:31</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -614,33 +606,29 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Variasi: Kipas bunga rotan</t>
+          <t>Variasi: Mangkok sambal tutup</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Ketebalan: tebalKualitas: okDesain: menarikSsuai gmbr &amp; keterangan
-produk baik &amp; brmutu
-respon &amp; pengiriman cepat
-packing aman &amp; bgs
-Penjual amanah &amp; tr prcya</t>
+          <t>Desain: menarik dan modernWarna: menarik dan ceriaKetebalan: lumayan tebalAlhamdulillah barang nya sdh sampai dengan baik dan benar,, real picture bagus mangkuk sambel nya,,untuk harga segitu mah wort it,,terima kasih. Desain: menarik dan modern. Warna: menarik dan ceria. Ketebalan: lumayan tebal. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, real picture bagus mangkuk sambel nya,,untuk harga segitu mah wort it,,terima kasih</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Rak Mini segi susun 3 Flower - Rak bumbu kosmetik serbagunaVariasi: Rak segi Flower</t>
+          <t>(10bks) korek batang kayu jadul gambar grosirVariasi: 10bks korek pelangi</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>/Rak-Mini-segi-susun-3-Flower-Rak-bumbu-kosmetik-serbaguna-i.145589728.21491056248</t>
+          <t>/(10bks)-korek-batang-kayu-jadul-gambar-grosir-i.145589728.11483476549</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-05-25 01:08</t>
+          <t>2025-05-25 13:31</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -648,433 +636,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Variasi: Rak segi Flower</t>
+          <t>Variasi: 10bks korek pelangi</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Mohon lebih d tingkatkan lg pelayanannya agar lebih teliti.. Makasih barang2 nya murah² tp berkualitas sayang nya jauh banget klo dr tempt aku mh jd ongkirnya mahal banget walaupun sdh dapet voucer gratis . Sukses terus 👍</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>(1pcs) Centong entong nasi plastik tebal warna dx termurahVariasi: Ecer_1bj centong PLG</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>/(1pcs)-Centong-entong-nasi-plastik-tebal-warna-dx-termurah-i.145589728.2821981447</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2025-05-25 00:17</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Variasi: Ecer_1bj centong PLG</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Ketebalan: penipuDesain: penipuKualitas: penipuada 3 barang gk di kirim .. dan di paket tetep bayar full .. di chat gk di bales" .. emang sering nipu kali ni toko .. tolong yg lain mending beli di toko oren yg lain aja biar gk ketipu juga</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Gelas stand dudukan gelas oval capucino isi 6 gelas plastikVariasi: Gelas Stand Coklat</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>/Gelas-stand-dudukan-gelas-oval-capucino-isi-6-gelas-plastik-i.145589728.19090884439</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2025-05-24 23:51</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Variasi: Gelas Stand Coklat</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Desain: bagusKualitas Bahan: okInstalasi: mudahSangat rekomended untuk langganan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosirVariasi: Hngr benmore coklat</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2025-05-24 23:23</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>5</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Variasi: Hngr benmore coklat</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Barang sesuai pesanan.. dikemas cepat.. pengiriman cepat ,exp lama</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Tong sampah segi kicik hitam 5 liter kecil persegi plastik tebalVariasi: TS. Kicik 5L HITAM,Isi 1 pcs</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>/Tong-sampah-segi-kicik-hitam-5-liter-kecil-persegi-plastik-tebal-i.145589728.25059427941</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2025-05-24 23:21</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>5</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Variasi: TS. Kicik 5L HITAM,Isi 1 pcs</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Desain: TopUkuran: TOPKualitas Bahan: tOPtop</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Piring seng enamel lurik ukuran 22 cm besar tebal merk TBVariasi: Piring seng lurik,22cm Besar</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>/Piring-seng-enamel-lurik-ukuran-22-cm-besar-tebal-merk-TB-i.145589728.18783036648</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2025-05-24 22:59</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>5</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Variasi: Piring seng lurik,22cm Besar</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Ketebalan: sedangDesain: jaduuuullllllKualitas: baikTerima kasih barang sudah sampai dan sesuai</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Termos Capucino 6L dan 8L - Rice Ice bucket ekomonis grosirVariasi: Termos eknomis 6L</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>/Termos-Capucino-6L-dan-8L-Rice-Ice-bucket-ekomonis-grosir-i.145589728.29500951143</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2025-05-24 22:15</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>5</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Variasi: Termos eknomis 6L</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Ukuran: imut imutDesain: bagus warna sesuai picKondisi: dalam kondisi baikTerimakasih seller dan shopee</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Kursi jongkok CM Abu-abu warna tebal serbaguna - kursi duduk dapur kokohVariasi: Kursi abu ONIX</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>/Kursi-jongkok-CM-Abu-abu-warna-tebal-serbaguna-kursi-duduk-dapur-kokoh-i.145589728.7958001380</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2025-05-24 21:01</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>5</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Variasi: Kursi abu ONIX</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Bagus</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>kapstok baju stainless 6 kait - gantungan baju stainless muranVariasi: Kapstok jempol_6</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>/kapstok-baju-stainless-6-kait-gantungan-baju-stainless-muran-i.145589728.6442847024</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2025-05-24 20:37</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>5</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Variasi: Kapstok jempol_6</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Desain: eleganDurabilitas: sangat bagusKualitas Bahan: kuat</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Botol saos kecap memeclub tinggi 400 ml plastik grosirVariasi: Meme club tinggi</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>/Botol-saos-kecap-memeclub-tinggi-400-ml-plastik-grosir-i.145589728.3913320949</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>2025-05-24 20:00</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>5</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Variasi: Meme club tinggi</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Desain: bagusWarna: sesuaiKualitas: bagus</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>kapstok baju stainless 6 kait - gantungan baju stainless muranVariasi: Kapstok jempol_6</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>/kapstok-baju-stainless-6-kait-gantungan-baju-stainless-muran-i.145589728.6442847024</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>2025-05-24 19:59</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>5</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Variasi: Kapstok jempol_6</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Desain: bagusDurabilitas: okKualitas Bahan: kuatPuas dengan pesanan saya 
-Sesuai gambar.,.</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>(12pcs) Cetakan roti kukus bentuk love rege cerah plastik dxVariasi: 12BJ Ctkn LOVE</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>/(12pcs)-Cetakan-roti-kukus-bentuk-love-rege-cerah-plastik-dx-i.145589728.15424268542</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2025-05-24 19:49</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>5</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Variasi: 12BJ Ctkn LOVE</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Alhamdulillah paketku sampai dg selamat,barangnya bagus sesuai pict..makasih kak</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>(12pak) Cotten bud - cotton bud motif bunga halus dan lembut grosirVariasi: 1pak cotenbud bunga</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>/(12pak)-Cotten-bud-cotton-bud-motif-bunga-halus-dan-lembut-grosir-i.145589728.16880893501</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2025-05-24 19:45</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>5</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Variasi: 1pak cotenbud bunga</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Cocok untuk: semuaKapasitas: bagusKualitas: aman</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Mangkok stainless 14 cm 16 cm tebal - baskom stainless serbaguna grosirVariasi: Mangkok 16 cm</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>/Mangkok-stainless-14-cm-16-cm-tebal-baskom-stainless-serbaguna-grosir-i.145589728.10650960952</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>2025-05-24 19:45</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>5</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Variasi: Mangkok 16 cm</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Ukuran: yang di harapkanKualitas Bahan: bagusDurabilitas: kokoh</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Tambahan packing kardus paket tambahan agar safetyVariasi: Kardus saftey</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>/Tambahan-packing-kardus-paket-tambahan-agar-safety-i.145589728.6615737043</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>2025-05-24 19:45</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>5</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Variasi: Kardus saftey</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Ketebalan: aman</t>
+          <t>Desain: menarikKualitas: kemasan nya baikKeaslian: asli korekAlhamdulillah barang nya sdh sampai dengan baik,,pesan yg pelangu datang nya yg biasa,,gpp tp dpt tambahan korek gas nya. Desain: menarik. Kualitas: kemasan nya baik. Keaslian: asli korek. Alhamdulillah barang nya sdh sampai dengan baik,,pesan yg pelangu datang nya yg biasa,,gpp tp dpt tambahan korek gas nya</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance review text extraction in scraping2.py for better clarity and accuracy. Update hns.csv to reflect improved review formatting and add missing product entries. Modify hns.xlsx to align with the latest data changes.
</commit_message>
<xml_diff>
--- a/hns.xlsx
+++ b/hns.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Desain: menarikKualitas Bahan: tebalKualitas: baiktempat minyak nya bagus bahannya tebal kualitas nya baik muat 2 liter minyak. Desain: menarik. Kualitas Bahan: tebal. Kualitas: baik. tempat minyak nya bagus bahannya tebal kualitas nya baik muat 2 liter minyak</t>
+          <t>menarik. tebal. baik. tempat minyak nya bagus bahannya tebal kualitas nya baik muat 2 liter minyak</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Ukuran: pasDesain: bagusDurabilitas: kuat dan kokoh. Ukuran: pas. Desain: bagus. Durabilitas: kuat dan kokoh</t>
+          <t>pas. bagus. kuat dan kokoh</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Ukuran: pas sesuai gambarKetebalan: ok tebalDurabilitas: produk sangat kuat. Ukuran: pas sesuai gambar. Ketebalan: ok tebal. Durabilitas: produk sangat kuat</t>
+          <t>pas sesuai gambar. ok tebal. produk sangat kuat</t>
         </is>
       </c>
     </row>
@@ -611,37 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Desain: menarik dan modernWarna: menarik dan ceriaKetebalan: lumayan tebalAlhamdulillah barang nya sdh sampai dengan baik dan benar,, real picture bagus mangkuk sambel nya,,untuk harga segitu mah wort it,,terima kasih. Desain: menarik dan modern. Warna: menarik dan ceria. Ketebalan: lumayan tebal. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, real picture bagus mangkuk sambel nya,,untuk harga segitu mah wort it,,terima kasih</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>(10bks) korek batang kayu jadul gambar grosirVariasi: 10bks korek pelangi</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>/(10bks)-korek-batang-kayu-jadul-gambar-grosir-i.145589728.11483476549</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-05-25 13:31</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Variasi: 10bks korek pelangi</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Desain: menarikKualitas: kemasan nya baikKeaslian: asli korekAlhamdulillah barang nya sdh sampai dengan baik,,pesan yg pelangu datang nya yg biasa,,gpp tp dpt tambahan korek gas nya. Desain: menarik. Kualitas: kemasan nya baik. Keaslian: asli korek. Alhamdulillah barang nya sdh sampai dengan baik,,pesan yg pelangu datang nya yg biasa,,gpp tp dpt tambahan korek gas nya</t>
+          <t>menarik dan modern. menarik dan ceria. lumayan tebal. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, real picture bagus mangkuk sambel nya,,untuk harga segitu mah wort it,,terima kasih</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refine product name extraction in scraping2.py by removing variation details. Update hns.csv with new product entries and ensure hns.xlsx is consistent with the latest data changes.
</commit_message>
<xml_diff>
--- a/hns.xlsx
+++ b/hns.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oil Jug tempat minyak sally 2 Liter plastik + TutupVariasi: Oil jug SALLY 2L</t>
+          <t>Oil Jug tempat minyak sally 2 Liter plastik + Tutup</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -498,7 +498,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rak Mini segi susun 3 Flower - Rak bumbu kosmetik serbagunaVariasi: Rak segi Flower</t>
+          <t>Rak Mini segi susun 3 Flower - Rak bumbu kosmetik serbaguna</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -528,7 +528,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Rak plastik serbaguna susun 3 lovina warna goldVariasi: Rak lovina Gold</t>
+          <t>Rak plastik serbaguna susun 3 lovina warna gold</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Silet cukur tatra original extra tajam 10 pcs - silet serbagunaVariasi: Silet tatra</t>
+          <t>Silet cukur tatra original extra tajam 10 pcs - silet serbaguna</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -588,7 +588,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mangko sambal bakso tutup panda star plus sendok bulat oval plastikVariasi: Mangkok sambal tutup</t>
+          <t>Mangko sambal bakso tutup panda star plus sendok bulat oval plastik</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -612,6 +612,96 @@
       <c r="F6" t="inlineStr">
         <is>
           <t>menarik dan modern. menarik dan ceria. lumayan tebal. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, real picture bagus mangkuk sambel nya,,untuk harga segitu mah wort it,,terima kasih</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>(10bks) korek batang kayu jadul gambar grosir</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>/(10bks)-korek-batang-kayu-jadul-gambar-grosir-i.145589728.11483476549</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-05-25 13:31</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Variasi: 10bks korek pelangi</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>menarik. kemasan nya baik. asli korek. Alhamdulillah barang nya sdh sampai dengan baik,,pesan yg pelangu datang nya yg biasa,,gpp tp dpt tambahan korek gas nya</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>(12pcs) Solet pelet kue plastik Nice spatula murah serbaguna grosir</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>/(12pcs)-Solet-pelet-kue-plastik-Nice-spatula-murah-serbaguna-grosir-i.145589728.3613664874</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-05-25 13:31</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Variasi: 12bj solet kecil</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>warna produk sesuai deskripsi. menggunakan bahan yg bagus dan awet. sangat awet dan tahan lama. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, sesuai dengan deskripsi,, pengiriman nya sangat cepat,,</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>erus Irus motif jagung kecil kuah sayur sendok sayutr satinless steel murah berkualitas</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>/erus-Irus-motif-jagung-kecil-kuah-sayur-sendok-sayutr-satinless-steel-murah-berkualitas-i.145589728.6042850355</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-05-25 13:21</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Variasi: Irus jagung kecil</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>baguz. imut. bagus. Oke deh bagus ,boleh deh kpan² belanja lagi di toko ini</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Increase target review count in scraping2.py to 600 and enhance review text filtering logic for improved data quality. Update hns.csv with additional product entries and ensure hns.xlsx is synchronized with the latest changes.
</commit_message>
<xml_diff>
--- a/hns.xlsx
+++ b/hns.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,17 +468,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oil Jug tempat minyak sally 2 Liter plastik + Tutup</t>
+          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosir</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>/Oil-Jug-tempat-minyak-sally-2-Liter-plastik-Tutup-i.145589728.23248604754</t>
+          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-05-25 14:12</t>
+          <t>2025-05-25 14:32</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -486,29 +486,29 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Variasi: Oil jug SALLY 2L</t>
+          <t>Variasi: Hngr benmore coklat</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>menarik. tebal. baik. tempat minyak nya bagus bahannya tebal kualitas nya baik muat 2 liter minyak</t>
+          <t>Pengemasan bagus, jadi aman sampai tujuan, kualitasnya juga bagus, worth it to buy</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rak Mini segi susun 3 Flower - Rak bumbu kosmetik serbaguna</t>
+          <t>Oil Jug tempat minyak sally 2 Liter plastik + Tutup</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>/Rak-Mini-segi-susun-3-Flower-Rak-bumbu-kosmetik-serbaguna-i.145589728.21491056248</t>
+          <t>/Oil-Jug-tempat-minyak-sally-2-Liter-plastik-Tutup-i.145589728.23248604754</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-05-25 14:10</t>
+          <t>2025-05-25 14:12</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,29 +516,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Variasi: Rak segi Flower</t>
+          <t>Variasi: Oil jug SALLY 2L</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>pas. bagus. kuat dan kokoh</t>
+          <t>menarik. tebal. baik. tempat minyak nya bagus bahannya tebal kualitas nya baik muat 2 liter minyak</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Rak plastik serbaguna susun 3 lovina warna gold</t>
+          <t>Rak Mini segi susun 3 Flower - Rak bumbu kosmetik serbaguna</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>/Rak-plastik-serbaguna-susun-3-lovina-warna-gold-i.145589728.24033169934</t>
+          <t>/Rak-Mini-segi-susun-3-Flower-Rak-bumbu-kosmetik-serbaguna-i.145589728.21491056248</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-05-25 14:05</t>
+          <t>2025-05-25 14:10</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -546,84 +546,84 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Variasi: Rak lovina Gold</t>
+          <t>Variasi: Rak segi Flower</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>pas sesuai gambar. ok tebal. produk sangat kuat</t>
+          <t>pas. bagus. kuat dan kokoh</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Silet cukur tatra original extra tajam 10 pcs - silet serbaguna</t>
+          <t>Rak plastik serbaguna susun 3 lovina warna gold</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>/Silet-cukur-tatra-original-extra-tajam-10-pcs-silet-serbaguna-i.145589728.9915872611</t>
+          <t>/Rak-plastik-serbaguna-susun-3-lovina-warna-gold-i.145589728.24033169934</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-05-25 14:00</t>
+          <t>2025-05-25 14:05</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Variasi: Silet tatra</t>
+          <t>Variasi: Rak lovina Gold</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Produk sudah sampai sesuai dengan pesanan terimakasihhhh</t>
+          <t>pas sesuai gambar. ok tebal. produk sangat kuat</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mangko sambal bakso tutup panda star plus sendok bulat oval plastik</t>
+          <t>Silet cukur tatra original extra tajam 10 pcs - silet serbaguna</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>/Mangko-sambal-bakso-tutup-panda-star-plus-sendok-bulat-oval-plastik-i.145589728.16385939181</t>
+          <t>/Silet-cukur-tatra-original-extra-tajam-10-pcs-silet-serbaguna-i.145589728.9915872611</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-05-25 13:31</t>
+          <t>2025-05-25 14:00</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Variasi: Mangkok sambal tutup</t>
+          <t>Variasi: Silet tatra</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>menarik dan modern. menarik dan ceria. lumayan tebal. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, real picture bagus mangkuk sambel nya,,untuk harga segitu mah wort it,,terima kasih</t>
+          <t>Produk sudah sampai sesuai dengan pesanan terimakasihhhh</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>(10bks) korek batang kayu jadul gambar grosir</t>
+          <t>Mangko sambal bakso tutup panda star plus sendok bulat oval plastik</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>/(10bks)-korek-batang-kayu-jadul-gambar-grosir-i.145589728.11483476549</t>
+          <t>/Mangko-sambal-bakso-tutup-panda-star-plus-sendok-bulat-oval-plastik-i.145589728.16385939181</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -636,24 +636,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Variasi: 10bks korek pelangi</t>
+          <t>Variasi: Mangkok sambal tutup</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>menarik. kemasan nya baik. asli korek. Alhamdulillah barang nya sdh sampai dengan baik,,pesan yg pelangu datang nya yg biasa,,gpp tp dpt tambahan korek gas nya</t>
+          <t>menarik dan modern. menarik dan ceria. lumayan tebal. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, real picture bagus mangkuk sambel nya,,untuk harga segitu mah wort it,,terima kasih</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>(12pcs) Solet pelet kue plastik Nice spatula murah serbaguna grosir</t>
+          <t>(10bks) korek batang kayu jadul gambar grosir</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>/(12pcs)-Solet-pelet-kue-plastik-Nice-spatula-murah-serbaguna-grosir-i.145589728.3613664874</t>
+          <t>/(10bks)-korek-batang-kayu-jadul-gambar-grosir-i.145589728.11483476549</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -666,42 +666,1602 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Variasi: 12bj solet kecil</t>
+          <t>Variasi: 10bks korek pelangi</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>warna produk sesuai deskripsi. menggunakan bahan yg bagus dan awet. sangat awet dan tahan lama. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, sesuai dengan deskripsi,, pengiriman nya sangat cepat,,</t>
+          <t>menarik. kemasan nya baik. asli korek. Alhamdulillah barang nya sdh sampai dengan baik,,pesan yg pelangu datang nya yg biasa,,gpp tp dpt tambahan korek gas nya</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>(12pcs) Solet pelet kue plastik Nice spatula murah serbaguna grosir</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>/(12pcs)-Solet-pelet-kue-plastik-Nice-spatula-murah-serbaguna-grosir-i.145589728.3613664874</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-05-25 13:31</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Variasi: 12bj solet kecil</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>warna produk sesuai deskripsi. menggunakan bahan yg bagus dan awet. sangat awet dan tahan lama. Alhamdulillah barang nya sdh sampai dengan baik dan benar,, sesuai dengan deskripsi,, pengiriman nya sangat cepat,,</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>erus Irus motif jagung kecil kuah sayur sendok sayutr satinless steel murah berkualitas</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>/erus-Irus-motif-jagung-kecil-kuah-sayur-sendok-sayutr-satinless-steel-murah-berkualitas-i.145589728.6042850355</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>2025-05-25 13:21</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>Variasi: Irus jagung kecil</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>baguz. imut. bagus. Oke deh bagus ,boleh deh kpan² belanja lagi di toko ini</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Termos Capucino 6L dan 8L - Rice Ice bucket ekomonis grosir</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>/Termos-Capucino-6L-dan-8L-Rice-Ice-bucket-ekomonis-grosir-i.145589728.29500951143</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-05-25 13:14</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Variasi: Termos ekonomis 8L</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Real pict</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tutup cangkir stainless  8 cm dan per 1 biji - tutup gelas murah berkualitas</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>/Tutup-cangkir-stainless-8-cm-dan-per-1-biji-tutup-gelas-murah-berkualitas-i.145589728.4552724536</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:58</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Variasi: Ttp GLS Stainls KCL</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>kurang. D penyok pd potol jg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosir</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:48</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Variasi: Hngr benmore coklat</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Tipis banget sesuai harga</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Keranjang surat DNP panjang model perahu serbaguna plastik</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>/Keranjang-surat-DNP-panjang-model-perahu-serbaguna-plastik-i.145589728.10637069354</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:39</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Variasi: Krnjng surat perahu</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Terima kasih barangnya sudah sampai dengan aman dan terkendali,,</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Tempat sendok alat tulis gandeng moly coklat grosir</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>/Tempat-sendok-alat-tulis-gandeng-moly-coklat-grosir-i.145589728.29314709869</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:37</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Variasi: Tempat sendok moly</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>barang datang pecah kak</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>erus Irus motif jagung kecil kuah sayur sendok sayutr satinless steel murah berkualitas</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>/erus-Irus-motif-jagung-kecil-kuah-sayur-sendok-sayutr-satinless-steel-murah-berkualitas-i.145589728.6042850355</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:37</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Variasi: Irus jagung kecil</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Pengaman regulator - pengunci penahan regulator tabung gas 3 kg dan 12 kg</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>/Pengaman-regulator-pengunci-penahan-regulator-tabung-gas-3-kg-dan-12-kg-i.145589728.2408393733</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:32</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Variasi: Pengaman</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Tokonya SGT amanah, MW order lagi untk yg kedua kalinya</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>(1pcs) Centong entong nasi plastik tebal warna dx termurah</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>/(1pcs)-Centong-entong-nasi-plastik-tebal-warna-dx-termurah-i.145589728.2821981447</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:29</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Variasi: Ecer_1bj centong PLG</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>barang yg terkirim kurang 1 nacam gelas tutup gagang tidak di kirim</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosir</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:23</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>5</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Variasi: Hngr benmore coklat</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>baik. baik suka sekali sangat sangat pas dan cocok sekali</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>(12bj) cetakan puding jelly bunga melati kukus plastik warna dx rainbow</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>/(12bj)-cetakan-puding-jelly-bunga-melati-kukus-plastik-warna-dx-rainbow-i.145589728.13565673634</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-05-25 12:23</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Variasi: 12bj ctakn Melati</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>bagus. terang. bahannya tebal,seperti bukan dari plastik daur ulang. Rekomendet</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>(1pak) lilin cakra besar panjang 15 cm per pak 8 bj - Lilin putih grosir</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>/(1pak)-lilin-cakra-besar-panjang-15-cm-per-pak-8-bj-Lilin-putih-grosir-i.145589728.13613651443</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:54</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Variasi: 1pak lilin cakra</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>barang banyak pecah</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosir</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:54</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Variasi: Hngr benmore coklat</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>ok. Terikirim dg baik, aman. semoga awet thankyou seller</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Bukut tabungan murah isi 12 halaman warna warni grosir</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>/Bukut-tabungan-murah-isi-12-halaman-warna-warni-grosir-i.145589728.28114680452</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:54</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Variasi: Buku tabungan</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Fungsi:. ok. Konten:. Penampilan:. Thanks seller</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Saringan sayur manila plastik serbaguna diameter 20 cm tebal tidak mudah robek</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>/Saringan-sayur-manila-plastik-serbaguna-diameter-20-cm-tebal-tidak-mudah-robek-i.145589728.11240734388</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:54</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>5</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Variasi: Saringan sayur</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>tebal. semoga awet. kokoh. No cacat packingan oke sampai dg aman terimakasih</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Jepit baju pakaian laundry clip ABG jepitan jemuran per 20 pcs termurah</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>/Jepit-baju-pakaian-laundry-clip-ABG-jepitan-jemuran-per-20-pcs-termurah-i.145589728.7837312797</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:54</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>5</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Variasi: Jepit_Abg</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>ok. random. Sampai dg aman dan sesuai pesanan thanks seller</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosir</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:42</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>5</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Variasi: Hngr benmore coklat</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>lucu. pas. bagus. Murce bgt, dgn harga segini.🥰 makasih seller</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>(12 pcs) Tutup gelas biasa bahan plastik murah grosir berkualitas</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>/(12-pcs)-Tutup-gelas-biasa-bahan-plastik-murah-grosir-berkualitas-i.145589728.4439451825</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:39</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>5</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Variasi: 12bj_ttp gelas biasa</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>lucu. tebal. kualitas top. Bagus , harga ekonomis dan cocok untuk usaha warkop</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Hanger kawat briliant dewasa per 10 pcs panjang 35 cm anti karat</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>/Hanger-kawat-briliant-dewasa-per-10-pcs-panjang-35-cm-anti-karat-i.145589728.4937998304</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:39</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>5</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Variasi: Hanger briliant</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>menarik. aterial sangat bagus. pas dan sesuai ekspetasi. pokok e bagus</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Cangkir gelas minum plastik gmc gelas bir gagang grosir</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>/Cangkir-gelas-minum-plastik-gmc-gelas-bir-gagang-grosir-i.145589728.5581664849</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-05-25 11:32</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>5</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Variasi: Gelas bir plastik</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>bagud. cukup tebal. bagus. bagus sipp</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosir</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-05-25 10:55</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>5</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Variasi: Hngr benmore coklat</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Bagus sesuai harga barangnya. Mayan lah buat tambah² disaat cucian bnyak. Satu melengkung karna posisi di packaging nya tidak benar tapi it's oke kok</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Jepit baju pakaian laundry clip ABG jepitan jemuran per 20 pcs termurah</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>/Jepit-baju-pakaian-laundry-clip-ABG-jepitan-jemuran-per-20-pcs-termurah-i.145589728.7837312797</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-05-25 10:55</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>5</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Variasi: Jepit_Abg</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Bagus dan sesuai. Jepitnya cakep warnanya cerah, next bakal order lagi sih. Pengiriman juga cepet, recommended</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>(1pak) lilin cakra besar panjang 15 cm per pak 8 bj - Lilin putih grosir</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>/(1pak)-lilin-cakra-besar-panjang-15-cm-per-pak-8-bj-Lilin-putih-grosir-i.145589728.13613651443</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-05-25 10:44</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Variasi: 1pk lilin panda</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>kecil,katanya besar</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>(12 pcs) lap serbet dapur warna warni besar tebal kotak kotak 51x51 cm - grosir lap dapur warna</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>/(12-pcs)-lap-serbet-dapur-warna-warni-besar-tebal-kotak-kotak-51x51-cm-grosir-lap-dapur-warna-i.145589728.4834377203</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-05-25 09:26</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>4</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Variasi: 12bj Lap_warna</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Tipis tipis tipis</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Kamper rentengan putih - kapur barus 1 renteng isi 24 pcs</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>/Kamper-rentengan-putih-kapur-barus-1-renteng-isi-24-pcs-i.145589728.25659137417</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-05-25 09:20</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>5</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Variasi: 24BJ KAMPER</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Aroma:. baik. kemasan plastik untuk dijual kembali</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Hanger anak plastik benmore 1 pak isi 6pcs grosir</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>/Hanger-anak-plastik-benmore-1-pak-isi-6pcs-grosir-i.145589728.28414764389</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-05-25 09:14</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>5</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Variasi: Hngr benmore coklat</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Suka banget sama bahan nya tebel untuk harga segitu makasi seller</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Jepit baju pakaian laundry clip ABG jepitan jemuran per 20 pcs termurah</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>/Jepit-baju-pakaian-laundry-clip-ABG-jepitan-jemuran-per-20-pcs-termurah-i.145589728.7837312797</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-05-25 09:03</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>5</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Variasi: Jepit_Abg</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Semua bagus</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>(1Rtng) Jarum jahitan set piring bulat - Jarum renten kemasan isi 12 bj per renteng</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>/(1Rtng)-Jarum-jahitan-set-piring-bulat-Jarum-renten-kemasan-isi-12-bj-per-renteng-i.145589728.29320101679</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-05-25 08:56</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>4</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Variasi: 12BJ JARUM PIRING</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Barang sudah diterima produk bagus tapi kurang barangnya 1pcs, gak jujur kurang amanah, ok terimakasih shopee dan kurirnya</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Kamper rentengan putih - kapur barus 1 renteng isi 24 pcs</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>/Kamper-rentengan-putih-kapur-barus-1-renteng-isi-24-pcs-i.145589728.25659137417</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-05-25 08:56</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>5</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Variasi: 24BJ KAMPER</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Barang sudah diterima produk bagus sesuai harapan terimakasih semuanya</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>(24bks) Peniti putih rentengan semua ukuran murah grosir</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>/(24bks)-Peniti-putih-rentengan-semua-ukuran-murah-grosir-i.145589728.11825723727</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-05-25 08:56</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>5</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Variasi: 24bks peniti putih</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Barang sudah diterima produk bagus sesuai harapan tapi barangnya kurang juga satu pcs ok terimakasih shopee dan kurirnya</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Tambal lem panci bocor lakban aluminium foil kualitas super Per 24 pcs</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>/Tambal-lem-panci-bocor-lakban-aluminium-foil-kualitas-super-Per-24-pcs-i.145589728.5661297440</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-05-25 08:56</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>5</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Variasi: Lusinan lem panci</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Barang sudah diterima produk bagus sesuai harapan terimakasih semuanya</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Pengaman regulator tabung gas - penahan regulator</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>/Pengaman-regulator-tabung-gas-penahan-regulator-i.145589728.2340272635</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2025-05-25 08:56</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>5</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Variasi: Pengaman</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Barang sudah diterima produk bagus sesuai harapan terimakasih semuanya</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>(12pcs) Tutup gelas stainless 8cm berkualitas grosir</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>/(12pcs)-Tutup-gelas-stainless-8cm-berkualitas-grosir-i.145589728.27967769808</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2025-05-25 08:22</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Variasi: Tutup gelas stainles,Isi 12 BJ</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>tipis. penyok semua. Potensi Pasar:. ga layak jual normal. Barang rusak dari tokonya ga mungkin karena pengiriman rusaknya begini. Ini barang sortiran dijual.Pada penyok dan goresan bekas produksi. ga layak dijual di toko. Layak kalo dijual di loak. kalo jual beri keterangan klo itu bukan barang normal mulus yg layak pakai, itu barang BS sudah sortiran lecet2 semua</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Payung anak karkter murah diameter 64 cm - Payung anak grosir</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>/Payung-anak-karkter-murah-diameter-64-cm-Payung-anak-grosir-i.145589728.13515737192</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2025-05-25 08:17</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>5</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Variasi: Payung anak</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>cantik. Ketahanan:. lumayan. Cocok untuk:. hujan. Ternyata minimalis payung nya tapi pas d anak aku semoga awet tidak mudah rusak warna nya yang dikirim bagus pink dan ungu makasih seler makasih shopeee</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>(1pcs) Cangkir gelas plastik sawah AJ06 murah - cangkir serbaguna berkualitas</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>/(1pcs)-Cangkir-gelas-plastik-sawah-AJ06-murah-cangkir-serbaguna-berkualitas-i.145589728.3254386624</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2025-05-25 08:11</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>5</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Variasi: Cangkir sawah</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Barang oke👍👍👍</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Tambal lem panci bocor serbaguna - lakban almunium foill</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>/Tambal-lem-panci-bocor-serbaguna-lakban-almunium-foill-i.145589728.4737247784</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2025-05-25 07:25</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>5</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Variasi: 1 METER</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Paket sudah sampai. Lengkap sesuai pesanan. Terimakasih seller</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>(1toples) Kerokan rautan orotan pensil ukuran besar merk Vetro karakter</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>/(1toples)-Kerokan-rautan-orotan-pensil-ukuran-besar-merk-Vetro-karakter-i.145589728.20413971699</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2025-05-25 07:15</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>4</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Variasi: 1toples rautan</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Rautan di desk isi 24 , realnya cm 17 ndak penuh toplesnya</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Eskan fresia 3 liter plastik ceret minum bening motif bunga</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>/Eskan-fresia-3-liter-plastik-ceret-minum-bening-motif-bunga-i.145589728.8605964666</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2025-05-25 06:07</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>5</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Variasi: Eskan fresia</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>uk.kecil.sy pikir 3ltr itu besar ehtaunya datangnya malah kecil</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Rak plastik serbaguna susun 3 lovina warna gold</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>/Rak-plastik-serbaguna-susun-3-lovina-warna-gold-i.145589728.24033169934</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2025-05-25 04:40</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>5</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Variasi: Rak lovina Gold</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>pas dan sesuai</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Kapstok kawat vinil warna 6 gantungan - gantungan baju tempel kawat</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>/Kapstok-kawat-vinil-warna-6-gantungan-gantungan-baju-tempel-kawat-i.145589728.13014371227</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:44</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>5</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Variasi: Kapstok 6 warna</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Ssuai gmbr &amp; keterangan produk baik &amp; brmutu respon &amp; pengiriman cepat packing aman &amp; bgs Penjual amanah &amp; tr prcya</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Silet cukur tatra original extra tajam 10 pcs - silet serbaguna</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>/Silet-cukur-tatra-original-extra-tajam-10-pcs-silet-serbaguna-i.145589728.9915872611</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:44</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>5</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Variasi: Silet tatra</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Kandungan:. ok. Kenyamanan:. ck6. Efek:. blm dicoba. Ssuai gmbr &amp; keterangan produk baik &amp; brmutu respon &amp; pengiriman cepat packing aman &amp; bgs Penjual amanah &amp; tr prcya</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>kipas tangan plastik karakter waru murah warna warni</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>/kipas-tangan-plastik-karakter-waru-murah-warna-warni-i.145589728.5337255631</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:44</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>5</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Variasi: Kipas bunga rotan</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>tebal. ok. menarik. Ssuai gmbr &amp; keterangan produk baik &amp; brmutu respon &amp; pengiriman cepat packing aman &amp; bgs Penjual amanah &amp; tr prcya</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Rak Mini segi susun 3 Flower - Rak bumbu kosmetik serbaguna</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>/Rak-Mini-segi-susun-3-Flower-Rak-bumbu-kosmetik-serbaguna-i.145589728.21491056248</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>5</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Variasi: Rak segi Flower</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Mohon lebih d tingkatkan lg pelayanannya agar lebih teliti. Makasih barang2 nya murah² tp berkualitas sayang nya jauh banget klo dr tempt aku mh jd ongkirnya mahal banget walaupun sdh dapet voucer gratis . Sukses terus 👍</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Piring seng enamel lurik ukuran 22 cm besar tebal merk TB</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>/Piring-seng-enamel-lurik-ukuran-22-cm-besar-tebal-merk-TB-i.145589728.18783036648</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>5</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Variasi: Piring seng lurik,22cm Besar</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>0:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Cangkir mug enamel lurik dan polos ukuran 6 cm per 1 pcs</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>/Cangkir-mug-enamel-lurik-dan-polos-ukuran-6-cm-per-1-pcs-i.145589728.18295145195</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>5</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Variasi: Cangkir enamel 6cm,Lurik</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>0:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Folding kawat 24 stik - jemuran baju bayi kawat grosir</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>/Folding-kawat-24-stik-jemuran-baju-bayi-kawat-grosir-i.145589728.17807105620</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>5</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Variasi: Folding kawat</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>0:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Pasrah 4 in 1 besar parutan serbaguna plastik</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>/Pasrah-4-in-1-besar-parutan-serbaguna-plastik-i.145589728.16991300646</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>5</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Variasi: Pasrah besar 4in1</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>0:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>jarum pentul hijab bulat warna doff per 1 lempeng bulatan</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>/jarum-pentul-hijab-bulat-warna-doff-per-1-lempeng-bulatan-i.145589728.16752186213</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>5</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Variasi: Jarum pentul bulat</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>0:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>(2pcs) Baterai abc AAA kecil carbon zinc - Batrai murah grosir</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>/(2pcs)-Baterai-abc-AAA-kecil-carbon-zinc-Batrai-murah-grosir-i.145589728.11415856127</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>5</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Variasi: 2BJ ABC AAA MINI</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>0:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>(12pcs) Pen bulpen Bolpenku pen lilit spiral gel murah drhop technology</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>/(12pcs)-Pen-bulpen-Bolpenku-pen-lilit-spiral-gel-murah-drhop-technology-i.145589728.7516238456</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>5</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Variasi: 12bj bulpenku</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Parutan keju stainless steel murah grosir - parutan kentang sayur multiguna grosir Per PCS</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>/Parutan-keju-stainless-steel-murah-grosir-parutan-kentang-sayur-multiguna-grosir-Per-PCS-i.145589728.5410776566</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>5</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Variasi: Parutan keju</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>0:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Tatakan kompor rinnai kaki 4 glos - Dudukan kompor rinnai tebal</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>/Tatakan-kompor-rinnai-kaki-4-glos-Dudukan-kompor-rinnai-tebal-i.145589728.2273516291</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2025-05-25 01:08</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>5</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Variasi: Ttkan rinnai</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>0:10</t>
         </is>
       </c>
     </row>

</xml_diff>